<commit_message>
fix: created one simple integrated model for cohorts
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CohortsHarmonised.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CohortsHarmonised.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B22A198-A919-8748-9E56-86F2568FCCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF5AA61-AFA3-6142-88DA-5BED83A06D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="460" windowWidth="22080" windowHeight="17540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="108">
   <si>
     <t>name</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>values</t>
-  </si>
-  <si>
-    <t>topics</t>
   </si>
   <si>
     <t>value = label pairs</t>
@@ -805,7 +802,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,7 +839,7 @@
         <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>66</v>
@@ -905,13 +902,13 @@
         <v>76</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>51</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>71</v>
@@ -945,7 +942,7 @@
         <v>52</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K6" s="3" t="b">
         <v>1</v>
@@ -988,7 +985,7 @@
         <v>52</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>72</v>
@@ -1011,7 +1008,7 @@
         <v>52</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>73</v>
@@ -1028,7 +1025,7 @@
         <v>76</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>60</v>
@@ -1037,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1045,7 +1042,7 @@
         <v>76</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>60</v>
@@ -1054,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1062,13 +1059,13 @@
         <v>76</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K12" s="3" t="b">
         <v>1</v>
@@ -1173,7 +1170,7 @@
         <v>51</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>71</v>
@@ -1221,7 +1218,7 @@
     </row>
     <row r="21" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>0</v>
@@ -1238,7 +1235,7 @@
     </row>
     <row r="22" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>3</v>
@@ -1252,7 +1249,7 @@
     </row>
     <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>11</v>
@@ -1261,7 +1258,7 @@
         <v>51</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>75</v>
@@ -1275,7 +1272,7 @@
     </row>
     <row r="24" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>23</v>
@@ -1284,7 +1281,7 @@
         <v>51</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K24" s="10" t="b">
         <v>1</v>
@@ -1292,7 +1289,7 @@
     </row>
     <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>12</v>
@@ -1306,7 +1303,7 @@
     </row>
     <row r="26" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>13</v>
@@ -1320,7 +1317,7 @@
     </row>
     <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>0</v>
@@ -1337,7 +1334,7 @@
     </row>
     <row r="28" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>3</v>
@@ -1351,7 +1348,7 @@
     </row>
     <row r="29" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>16</v>
@@ -1365,7 +1362,7 @@
     </row>
     <row r="30" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>22</v>
@@ -1374,7 +1371,7 @@
         <v>51</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>22</v>
@@ -1385,7 +1382,7 @@
     </row>
     <row r="31" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>0</v>
@@ -1396,39 +1393,39 @@
     </row>
     <row r="32" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>50</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H32" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="J32" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="K32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="K32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>52</v>
@@ -1437,18 +1434,18 @@
         <v>1</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L33" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>6</v>
@@ -1459,24 +1456,24 @@
     </row>
     <row r="35" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>6</v>
       </c>
       <c r="L35" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>6</v>
@@ -1487,10 +1484,10 @@
     </row>
     <row r="37" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>17</v>
@@ -1552,7 +1549,7 @@
         <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>45</v>
@@ -1578,7 +1575,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1629,7 +1626,7 @@
         <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1652,7 +1649,7 @@
         <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1660,13 +1657,13 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1727,7 +1724,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1747,18 +1744,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
         <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>81</v>
@@ -1769,10 +1766,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1780,10 +1777,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>3</v>

</xml_diff>